<commit_message>
Implement more stopwords for ngrams
</commit_message>
<xml_diff>
--- a/data/Fakespeak-ENG/Analysis_output/press_release/Fakespeak_press_release_ngrams_headlines.xlsx
+++ b/data/Fakespeak-ENG/Analysis_output/press_release/Fakespeak_press_release_ngrams_headlines.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="644">
   <si>
     <t>n</t>
   </si>
@@ -183,64 +183,61 @@
     <t>new deal</t>
   </si>
   <si>
-    <t>we need</t>
-  </si>
-  <si>
-    <t>our oceans</t>
-  </si>
-  <si>
     <t>need blue</t>
   </si>
   <si>
     <t>blue new</t>
   </si>
   <si>
-    <t>your name</t>
-  </si>
-  <si>
-    <t>you agree</t>
-  </si>
-  <si>
-    <t>wisconsin they</t>
+    <t>wisconsin lost</t>
   </si>
   <si>
     <t>veterans speak</t>
   </si>
   <si>
-    <t>ve lost</t>
-  </si>
-  <si>
     <t>unprecedented opportunity</t>
   </si>
   <si>
     <t>trump promised</t>
   </si>
   <si>
-    <t>to rebuild</t>
-  </si>
-  <si>
-    <t>to pennsylvania</t>
-  </si>
-  <si>
-    <t>to deal</t>
-  </si>
-  <si>
-    <t>to bring</t>
-  </si>
-  <si>
-    <t>this year</t>
-  </si>
-  <si>
-    <t>the overwhelming</t>
-  </si>
-  <si>
-    <t>the necessary</t>
-  </si>
-  <si>
-    <t>the border</t>
-  </si>
-  <si>
-    <t>we need blue</t>
+    <t>speak gov</t>
+  </si>
+  <si>
+    <t>sen cruz</t>
+  </si>
+  <si>
+    <t>restore ocean</t>
+  </si>
+  <si>
+    <t>resources deal</t>
+  </si>
+  <si>
+    <t>republican veterans</t>
+  </si>
+  <si>
+    <t>rebuild blue</t>
+  </si>
+  <si>
+    <t>protect restore</t>
+  </si>
+  <si>
+    <t>promised bring</t>
+  </si>
+  <si>
+    <t>present unprecedented</t>
+  </si>
+  <si>
+    <t>people crossing</t>
+  </si>
+  <si>
+    <t>pennsylvania wisconsin</t>
+  </si>
+  <si>
+    <t>part fight</t>
+  </si>
+  <si>
+    <t>overwhelming influx</t>
   </si>
   <si>
     <t>need blue new</t>
@@ -249,175 +246,178 @@
     <t>blue new deal</t>
   </si>
   <si>
-    <t>your name if</t>
-  </si>
-  <si>
-    <t>you agree we</t>
-  </si>
-  <si>
-    <t>with the overwhelming</t>
-  </si>
-  <si>
-    <t>wisconsin they ve</t>
-  </si>
-  <si>
-    <t>veterans speak out</t>
-  </si>
-  <si>
-    <t>ve lost the</t>
-  </si>
-  <si>
-    <t>unprecedented opportunity to</t>
-  </si>
-  <si>
-    <t>trump promised to</t>
-  </si>
-  <si>
-    <t>to rebuild our</t>
-  </si>
-  <si>
-    <t>to pennsylvania and</t>
-  </si>
-  <si>
-    <t>to deal with</t>
-  </si>
-  <si>
-    <t>to bring jobs</t>
-  </si>
-  <si>
-    <t>to be key</t>
-  </si>
-  <si>
-    <t>they ve lost</t>
-  </si>
-  <si>
-    <t>the overwhelming influx</t>
-  </si>
-  <si>
-    <t>the necessary resources</t>
-  </si>
-  <si>
-    <t>the border illegally</t>
-  </si>
-  <si>
-    <t>we need blue new</t>
+    <t>wisconsin lost year</t>
+  </si>
+  <si>
+    <t>veterans speak gov</t>
+  </si>
+  <si>
+    <t>unprecedented opportunity key</t>
+  </si>
+  <si>
+    <t>trump promised bring</t>
+  </si>
+  <si>
+    <t>speak gov evers</t>
+  </si>
+  <si>
+    <t>sen cruz congress</t>
+  </si>
+  <si>
+    <t>restore ocean habitat</t>
+  </si>
+  <si>
+    <t>resources deal overwhelming</t>
+  </si>
+  <si>
+    <t>republican veterans speak</t>
+  </si>
+  <si>
+    <t>rebuild blue economy</t>
+  </si>
+  <si>
+    <t>protect restore ocean</t>
+  </si>
+  <si>
+    <t>promised bring jobs</t>
+  </si>
+  <si>
+    <t>present unprecedented opportunity</t>
+  </si>
+  <si>
+    <t>people crossing border</t>
+  </si>
+  <si>
+    <t>pennsylvania wisconsin lost</t>
+  </si>
+  <si>
+    <t>part fight climate</t>
+  </si>
+  <si>
+    <t>overwhelming influx people</t>
+  </si>
+  <si>
+    <t>opportunity key part</t>
   </si>
   <si>
     <t>need blue new deal</t>
   </si>
   <si>
-    <t>your name if you</t>
-  </si>
-  <si>
-    <t>you agree we need</t>
-  </si>
-  <si>
-    <t>with the overwhelming influx</t>
-  </si>
-  <si>
-    <t>wisconsin they ve lost</t>
-  </si>
-  <si>
-    <t>veterans speak out against</t>
-  </si>
-  <si>
-    <t>ve lost the most</t>
-  </si>
-  <si>
-    <t>unprecedented opportunity to be</t>
-  </si>
-  <si>
-    <t>trump promised to bring</t>
-  </si>
-  <si>
-    <t>to rebuild our blue</t>
-  </si>
-  <si>
-    <t>to pennsylvania and wisconsin</t>
-  </si>
-  <si>
-    <t>to deal with the</t>
-  </si>
-  <si>
-    <t>to bring jobs back</t>
-  </si>
-  <si>
-    <t>to be key part</t>
-  </si>
-  <si>
-    <t>they ve lost the</t>
-  </si>
-  <si>
-    <t>the overwhelming influx of</t>
-  </si>
-  <si>
-    <t>the necessary resources to</t>
-  </si>
-  <si>
-    <t>the most this year</t>
-  </si>
-  <si>
-    <t>speak out against gov</t>
-  </si>
-  <si>
-    <t>we need blue new deal</t>
-  </si>
-  <si>
-    <t>your name if you agree</t>
-  </si>
-  <si>
-    <t>you agree we need blue</t>
-  </si>
-  <si>
-    <t>with the overwhelming influx of</t>
-  </si>
-  <si>
-    <t>wisconsin they ve lost the</t>
-  </si>
-  <si>
-    <t>veterans speak out against gov</t>
-  </si>
-  <si>
-    <t>ve lost the most this</t>
-  </si>
-  <si>
-    <t>unprecedented opportunity to be key</t>
-  </si>
-  <si>
-    <t>trump promised to bring jobs</t>
-  </si>
-  <si>
-    <t>to rebuild our blue economy</t>
-  </si>
-  <si>
-    <t>to pennsylvania and wisconsin they</t>
-  </si>
-  <si>
-    <t>to deal with the overwhelming</t>
-  </si>
-  <si>
-    <t>to bring jobs back to</t>
-  </si>
-  <si>
-    <t>to be key part of</t>
-  </si>
-  <si>
-    <t>they ve lost the most</t>
-  </si>
-  <si>
-    <t>the overwhelming influx of people</t>
-  </si>
-  <si>
-    <t>the necessary resources to deal</t>
-  </si>
-  <si>
-    <t>speak out against gov evers</t>
+    <t>veterans speak gov evers</t>
+  </si>
+  <si>
+    <t>unprecedented opportunity key part</t>
+  </si>
+  <si>
+    <t>trump promised bring jobs</t>
+  </si>
+  <si>
+    <t>speak gov evers budget</t>
+  </si>
+  <si>
+    <t>sen cruz congress must</t>
+  </si>
+  <si>
+    <t>restore ocean habitat adapt</t>
+  </si>
+  <si>
+    <t>resources deal overwhelming influx</t>
+  </si>
+  <si>
+    <t>republican veterans speak gov</t>
+  </si>
+  <si>
+    <t>rebuild blue economy protect</t>
+  </si>
+  <si>
+    <t>protect restore ocean habitat</t>
+  </si>
+  <si>
+    <t>promised bring jobs back</t>
+  </si>
+  <si>
+    <t>present unprecedented opportunity key</t>
+  </si>
+  <si>
+    <t>people crossing border illegally</t>
+  </si>
+  <si>
+    <t>pennsylvania wisconsin lost year</t>
+  </si>
+  <si>
+    <t>part fight climate change</t>
+  </si>
+  <si>
+    <t>overwhelming influx people crossing</t>
+  </si>
+  <si>
+    <t>opportunity key part fight</t>
+  </si>
+  <si>
+    <t>oceans present unprecedented opportunity</t>
+  </si>
+  <si>
+    <t>oceans oceans present unprecedented</t>
+  </si>
+  <si>
+    <t>veterans speak gov evers budget</t>
+  </si>
+  <si>
+    <t>unprecedented opportunity key part fight</t>
+  </si>
+  <si>
+    <t>trump promised bring jobs back</t>
+  </si>
+  <si>
+    <t>speak gov evers budget proposal</t>
   </si>
   <si>
     <t>sen cruz congress must devote</t>
   </si>
   <si>
-    <t>restore ocean habitat and adapt</t>
+    <t>restore ocean habitat adapt climate</t>
+  </si>
+  <si>
+    <t>resources deal overwhelming influx people</t>
+  </si>
+  <si>
+    <t>republican veterans speak gov evers</t>
+  </si>
+  <si>
+    <t>rebuild blue economy protect restore</t>
+  </si>
+  <si>
+    <t>protect restore ocean habitat adapt</t>
+  </si>
+  <si>
+    <t>promised bring jobs back pennsylvania</t>
+  </si>
+  <si>
+    <t>present unprecedented opportunity key part</t>
+  </si>
+  <si>
+    <t>part fight climate change add</t>
+  </si>
+  <si>
+    <t>overwhelming influx people crossing border</t>
+  </si>
+  <si>
+    <t>opportunity key part fight climate</t>
+  </si>
+  <si>
+    <t>oceans present unprecedented opportunity key</t>
+  </si>
+  <si>
+    <t>oceans oceans present unprecedented opportunity</t>
+  </si>
+  <si>
+    <t>ocean habitat adapt climate changed</t>
+  </si>
+  <si>
+    <t>new deal rebuild blue economy</t>
+  </si>
+  <si>
+    <t>new deal oceans oceans present</t>
   </si>
   <si>
     <t>failed</t>
@@ -561,10 +561,7 @@
     <t>wilkes barre</t>
   </si>
   <si>
-    <t>while halting</t>
-  </si>
-  <si>
-    <t>tuition while</t>
+    <t>tuition halting</t>
   </si>
   <si>
     <t>trust patrick</t>
@@ -573,25 +570,10 @@
     <t>trump failed</t>
   </si>
   <si>
-    <t>to trust</t>
-  </si>
-  <si>
-    <t>to defund</t>
-  </si>
-  <si>
-    <t>to begin</t>
-  </si>
-  <si>
-    <t>to act</t>
-  </si>
-  <si>
-    <t>the wilkes</t>
-  </si>
-  <si>
     <t>testin republican</t>
   </si>
   <si>
-    <t>students during</t>
+    <t>students pandemic</t>
   </si>
   <si>
     <t>struggling citizen</t>
@@ -606,7 +588,7 @@
     <t>slams democrats</t>
   </si>
   <si>
-    <t>show me</t>
+    <t>show strong</t>
   </si>
   <si>
     <t>senate republican</t>
@@ -615,16 +597,31 @@
     <t>restore confidence</t>
   </si>
   <si>
-    <t>wisdems farmers have</t>
+    <t>response dragging</t>
+  </si>
+  <si>
+    <t>republican failure</t>
+  </si>
+  <si>
+    <t>republican conference</t>
+  </si>
+  <si>
+    <t>recovery plan</t>
+  </si>
+  <si>
+    <t>reasons trust</t>
+  </si>
+  <si>
+    <t>proposes defund</t>
+  </si>
+  <si>
+    <t>wisdems farmers crushed</t>
   </si>
   <si>
     <t>wilkes barre police</t>
   </si>
   <si>
-    <t>while halting applications</t>
-  </si>
-  <si>
-    <t>tuition while halting</t>
+    <t>tuition halting applications</t>
   </si>
   <si>
     <t>trust patrick testin</t>
@@ -633,55 +630,55 @@
     <t>trump failed covid</t>
   </si>
   <si>
-    <t>to trust patrick</t>
-  </si>
-  <si>
-    <t>to defund the</t>
-  </si>
-  <si>
-    <t>to begin may</t>
-  </si>
-  <si>
-    <t>to act costs</t>
-  </si>
-  <si>
-    <t>the wilkes barre</t>
-  </si>
-  <si>
     <t>testin republican failure</t>
   </si>
   <si>
-    <t>students during pandemic</t>
-  </si>
-  <si>
     <t>struggling citizen students</t>
   </si>
   <si>
     <t>strong recovery plan</t>
   </si>
   <si>
-    <t>state millions in</t>
-  </si>
-  <si>
-    <t>slams democrats for</t>
-  </si>
-  <si>
-    <t>show me strong</t>
+    <t>state millions federal</t>
+  </si>
+  <si>
+    <t>slams democrats giving</t>
+  </si>
+  <si>
+    <t>show strong recovery</t>
   </si>
   <si>
     <t>senate republican conference</t>
   </si>
   <si>
-    <t>restore confidence in</t>
-  </si>
-  <si>
-    <t>wisdems farmers have been</t>
-  </si>
-  <si>
-    <t>while halting applications for</t>
-  </si>
-  <si>
-    <t>tuition while halting applications</t>
+    <t>restore confidence elections</t>
+  </si>
+  <si>
+    <t>response dragging entire</t>
+  </si>
+  <si>
+    <t>republican failure act</t>
+  </si>
+  <si>
+    <t>republican conference slams</t>
+  </si>
+  <si>
+    <t>recovery plan begin</t>
+  </si>
+  <si>
+    <t>reasons trust patrick</t>
+  </si>
+  <si>
+    <t>proposes defund wilkes</t>
+  </si>
+  <si>
+    <t>plan begin may</t>
+  </si>
+  <si>
+    <t>wisdems farmers crushed trump</t>
+  </si>
+  <si>
+    <t>tuition halting applications struggling</t>
   </si>
   <si>
     <t>trust patrick testin republican</t>
@@ -690,58 +687,58 @@
     <t>trump failed covid 19</t>
   </si>
   <si>
-    <t>to trust patrick testin</t>
-  </si>
-  <si>
-    <t>to defund the wilkes</t>
-  </si>
-  <si>
-    <t>to act costs state</t>
-  </si>
-  <si>
-    <t>them down his entire</t>
-  </si>
-  <si>
-    <t>the wilkes barre police</t>
-  </si>
-  <si>
-    <t>testin republican failure to</t>
-  </si>
-  <si>
-    <t>struggling citizen students during</t>
-  </si>
-  <si>
-    <t>strong recovery plan to</t>
-  </si>
-  <si>
-    <t>state millions in federal</t>
-  </si>
-  <si>
-    <t>slams democrats for giving</t>
-  </si>
-  <si>
-    <t>show me strong recovery</t>
+    <t>testin republican failure act</t>
+  </si>
+  <si>
+    <t>struggling citizen students pandemic</t>
+  </si>
+  <si>
+    <t>strong recovery plan begin</t>
+  </si>
+  <si>
+    <t>state millions federal funds</t>
+  </si>
+  <si>
+    <t>slams democrats giving illegal</t>
+  </si>
+  <si>
+    <t>show strong recovery plan</t>
   </si>
   <si>
     <t>senate republican conference slams</t>
   </si>
   <si>
-    <t>restore confidence in our</t>
-  </si>
-  <si>
-    <t>response but he been</t>
-  </si>
-  <si>
-    <t>republican failure to act</t>
-  </si>
-  <si>
-    <t>wisdems farmers have been crushed</t>
-  </si>
-  <si>
-    <t>while halting applications for struggling</t>
-  </si>
-  <si>
-    <t>tuition while halting applications for</t>
+    <t>response dragging entire presidency</t>
+  </si>
+  <si>
+    <t>republican failure act costs</t>
+  </si>
+  <si>
+    <t>republican conference slams democrats</t>
+  </si>
+  <si>
+    <t>recovery plan begin may</t>
+  </si>
+  <si>
+    <t>reasons trust patrick testin</t>
+  </si>
+  <si>
+    <t>proposes defund wilkes barre</t>
+  </si>
+  <si>
+    <t>phase show strong recovery</t>
+  </si>
+  <si>
+    <t>patrick testin republican failure</t>
+  </si>
+  <si>
+    <t>parson announces first phase</t>
+  </si>
+  <si>
+    <t>wisdems farmers crushed trump failed</t>
+  </si>
+  <si>
+    <t>tuition halting applications struggling citizen</t>
   </si>
   <si>
     <t>trust patrick testin republican failure</t>
@@ -750,49 +747,52 @@
     <t>trump failed covid 19 response</t>
   </si>
   <si>
-    <t>to trust patrick testin republican</t>
-  </si>
-  <si>
-    <t>to defund the wilkes barre</t>
-  </si>
-  <si>
-    <t>to act costs state millions</t>
-  </si>
-  <si>
-    <t>them down his entire presidency</t>
-  </si>
-  <si>
-    <t>testin republican failure to act</t>
-  </si>
-  <si>
-    <t>struggling citizen students during pandemic</t>
-  </si>
-  <si>
-    <t>strong recovery plan to begin</t>
-  </si>
-  <si>
-    <t>state millions in federal funds</t>
-  </si>
-  <si>
-    <t>slams democrats for giving illegal</t>
-  </si>
-  <si>
-    <t>show me strong recovery plan</t>
+    <t>testin republican failure act costs</t>
+  </si>
+  <si>
+    <t>strong recovery plan begin may</t>
+  </si>
+  <si>
+    <t>slams democrats giving illegal immigrants</t>
+  </si>
+  <si>
+    <t>show strong recovery plan begin</t>
   </si>
   <si>
     <t>senate republican conference slams democrats</t>
   </si>
   <si>
-    <t>restore confidence in our elections</t>
-  </si>
-  <si>
-    <t>response but he been dragging</t>
-  </si>
-  <si>
-    <t>republican failure to act costs</t>
-  </si>
-  <si>
-    <t>republican conference slams democrats for</t>
+    <t>republican failure act costs state</t>
+  </si>
+  <si>
+    <t>republican conference slams democrats giving</t>
+  </si>
+  <si>
+    <t>reasons trust patrick testin republican</t>
+  </si>
+  <si>
+    <t>proposes defund wilkes barre police</t>
+  </si>
+  <si>
+    <t>phase show strong recovery plan</t>
+  </si>
+  <si>
+    <t>patrick testin republican failure act</t>
+  </si>
+  <si>
+    <t>parson announces first phase show</t>
+  </si>
+  <si>
+    <t>ny senate republican conference slams</t>
+  </si>
+  <si>
+    <t>million reasons trust patrick testin</t>
+  </si>
+  <si>
+    <t>immigrants free tuition halting applications</t>
+  </si>
+  <si>
+    <t>illegal immigrants free tuition halting</t>
   </si>
   <si>
     <t>scott</t>
@@ -951,16 +951,16 @@
     <t>weekly update</t>
   </si>
   <si>
-    <t>want to</t>
-  </si>
-  <si>
-    <t>votes no</t>
-  </si>
-  <si>
-    <t>votes against</t>
-  </si>
-  <si>
-    <t>violence as</t>
+    <t>want use</t>
+  </si>
+  <si>
+    <t>votes raising</t>
+  </si>
+  <si>
+    <t>votes pelosi</t>
+  </si>
+  <si>
+    <t>violence public</t>
   </si>
   <si>
     <t>video series</t>
@@ -969,10 +969,10 @@
     <t>use covid</t>
   </si>
   <si>
-    <t>update on</t>
-  </si>
-  <si>
-    <t>trip on</t>
+    <t>update biden</t>
+  </si>
+  <si>
+    <t>trip budget</t>
   </si>
   <si>
     <t>trillion payout</t>
@@ -981,19 +981,19 @@
     <t>treating gun</t>
   </si>
   <si>
-    <t>to use</t>
-  </si>
-  <si>
-    <t>to liberal</t>
-  </si>
-  <si>
-    <t>to choose</t>
-  </si>
-  <si>
-    <t>the price</t>
-  </si>
-  <si>
-    <t>the heritage</t>
+    <t>spending package</t>
+  </si>
+  <si>
+    <t>son daughter</t>
+  </si>
+  <si>
+    <t>seniors paying</t>
+  </si>
+  <si>
+    <t>scott issues</t>
+  </si>
+  <si>
+    <t>scott heritage</t>
   </si>
   <si>
     <t>sen rick scott</t>
@@ -1002,178 +1002,178 @@
     <t>biden inflation crisis</t>
   </si>
   <si>
-    <t>weekly update on</t>
-  </si>
-  <si>
-    <t>want to use</t>
-  </si>
-  <si>
-    <t>votes no on</t>
-  </si>
-  <si>
-    <t>votes against raising</t>
-  </si>
-  <si>
-    <t>violence as public</t>
+    <t>weekly update biden</t>
+  </si>
+  <si>
+    <t>want use covid</t>
+  </si>
+  <si>
+    <t>votes raising debt</t>
+  </si>
+  <si>
+    <t>votes pelosi trillion</t>
+  </si>
+  <si>
+    <t>violence public health</t>
   </si>
   <si>
     <t>use covid 19</t>
   </si>
   <si>
-    <t>update on biden</t>
-  </si>
-  <si>
-    <t>trip on budget</t>
+    <t>update biden inflation</t>
+  </si>
+  <si>
+    <t>trip budget video</t>
   </si>
   <si>
     <t>treating gun violence</t>
   </si>
   <si>
-    <t>to use covid</t>
-  </si>
-  <si>
-    <t>to liberal states</t>
-  </si>
-  <si>
-    <t>the price for</t>
-  </si>
-  <si>
-    <t>the heritage foundation</t>
-  </si>
-  <si>
-    <t>spending package as</t>
-  </si>
-  <si>
-    <t>seniors are paying</t>
+    <t>spending package payback</t>
+  </si>
+  <si>
+    <t>seniors paying price</t>
   </si>
   <si>
     <t>scott issues weekly</t>
   </si>
   <si>
+    <t>scott heritage foundation</t>
+  </si>
+  <si>
     <t>scott democrats want</t>
   </si>
   <si>
-    <t>scott and the</t>
-  </si>
-  <si>
-    <t>weekly update on biden</t>
-  </si>
-  <si>
-    <t>want to use covid</t>
-  </si>
-  <si>
-    <t>votes no on pelosi</t>
-  </si>
-  <si>
-    <t>votes against raising debt</t>
-  </si>
-  <si>
-    <t>violence as public health</t>
+    <t>scott america seniors</t>
+  </si>
+  <si>
+    <t>road trip budget</t>
+  </si>
+  <si>
+    <t>rick scott issues</t>
+  </si>
+  <si>
+    <t>rick scott heritage</t>
+  </si>
+  <si>
+    <t>weekly update biden inflation</t>
+  </si>
+  <si>
+    <t>want use covid 19</t>
+  </si>
+  <si>
+    <t>votes raising debt limit</t>
+  </si>
+  <si>
+    <t>votes pelosi trillion payout</t>
+  </si>
+  <si>
+    <t>violence public health crisis</t>
   </si>
   <si>
     <t>use covid 19 spending</t>
   </si>
   <si>
-    <t>update on biden inflation</t>
-  </si>
-  <si>
-    <t>trip on budget video</t>
-  </si>
-  <si>
-    <t>treating gun violence as</t>
-  </si>
-  <si>
-    <t>to use covid 19</t>
-  </si>
-  <si>
-    <t>the price for biden</t>
-  </si>
-  <si>
-    <t>the heritage foundation release</t>
-  </si>
-  <si>
-    <t>spending package as payback</t>
-  </si>
-  <si>
-    <t>seniors are paying the</t>
+    <t>update biden inflation crisis</t>
+  </si>
+  <si>
+    <t>trip budget video series</t>
+  </si>
+  <si>
+    <t>treating gun violence public</t>
+  </si>
+  <si>
+    <t>spending package payback liberal</t>
+  </si>
+  <si>
+    <t>seniors paying price biden</t>
   </si>
   <si>
     <t>sen rick scott issues</t>
   </si>
   <si>
+    <t>sen rick scott heritage</t>
+  </si>
+  <si>
     <t>sen rick scott democrats</t>
   </si>
   <si>
-    <t>sen rick scott and</t>
-  </si>
-  <si>
     <t>sen rick scott america</t>
   </si>
   <si>
     <t>scott issues weekly update</t>
   </si>
   <si>
-    <t>scott democrats want to</t>
-  </si>
-  <si>
-    <t>weekly update on biden inflation</t>
-  </si>
-  <si>
-    <t>want to use covid 19</t>
-  </si>
-  <si>
-    <t>votes no on pelosi trillion</t>
-  </si>
-  <si>
-    <t>votes against raising debt limit</t>
-  </si>
-  <si>
-    <t>violence as public health crisis</t>
+    <t>scott heritage foundation release</t>
+  </si>
+  <si>
+    <t>scott democrats want use</t>
+  </si>
+  <si>
+    <t>scott america seniors paying</t>
+  </si>
+  <si>
+    <t>road trip budget video</t>
+  </si>
+  <si>
+    <t>weekly update biden inflation crisis</t>
+  </si>
+  <si>
+    <t>want use covid 19 spending</t>
   </si>
   <si>
     <t>use covid 19 spending package</t>
   </si>
   <si>
-    <t>update on biden inflation crisis</t>
-  </si>
-  <si>
-    <t>trip on budget video series</t>
-  </si>
-  <si>
-    <t>treating gun violence as public</t>
-  </si>
-  <si>
-    <t>to use covid 19 spending</t>
-  </si>
-  <si>
-    <t>the price for biden inflation</t>
-  </si>
-  <si>
-    <t>the heritage foundation release episodes</t>
-  </si>
-  <si>
-    <t>spending package as payback to</t>
-  </si>
-  <si>
-    <t>seniors are paying the price</t>
+    <t>treating gun violence public health</t>
+  </si>
+  <si>
+    <t>spending package payback liberal states</t>
+  </si>
+  <si>
+    <t>seniors paying price biden inflation</t>
   </si>
   <si>
     <t>sen rick scott issues weekly</t>
   </si>
   <si>
+    <t>sen rick scott heritage foundation</t>
+  </si>
+  <si>
     <t>sen rick scott democrats want</t>
   </si>
   <si>
-    <t>sen rick scott and the</t>
-  </si>
-  <si>
     <t>sen rick scott america seniors</t>
   </si>
   <si>
-    <t>scott issues weekly update on</t>
-  </si>
-  <si>
-    <t>scott democrats want to use</t>
+    <t>scott issues weekly update biden</t>
+  </si>
+  <si>
+    <t>scott heritage foundation release episodes</t>
+  </si>
+  <si>
+    <t>scott democrats want use covid</t>
+  </si>
+  <si>
+    <t>scott america seniors paying price</t>
+  </si>
+  <si>
+    <t>road trip budget video series</t>
+  </si>
+  <si>
+    <t>rick scott issues weekly update</t>
+  </si>
+  <si>
+    <t>rick scott heritage foundation release</t>
+  </si>
+  <si>
+    <t>rick scott democrats want use</t>
+  </si>
+  <si>
+    <t>rick scott america seniors paying</t>
+  </si>
+  <si>
+    <t>release episodes road trip budget</t>
   </si>
   <si>
     <t>national</t>
@@ -1311,7 +1311,7 @@
     <t>white students</t>
   </si>
   <si>
-    <t>warrants as</t>
+    <t>warrants valid</t>
   </si>
   <si>
     <t>valid proof</t>
@@ -1320,25 +1320,13 @@
     <t>united states</t>
   </si>
   <si>
-    <t>tsa from</t>
+    <t>tsa accepting</t>
   </si>
   <si>
     <t>trump 45th</t>
   </si>
   <si>
-    <t>trends in</t>
-  </si>
-  <si>
-    <t>to prohibit</t>
-  </si>
-  <si>
-    <t>to hurt</t>
-  </si>
-  <si>
-    <t>the united</t>
-  </si>
-  <si>
-    <t>the commonwealt</t>
+    <t>trends national</t>
   </si>
   <si>
     <t>students persist</t>
@@ -1347,10 +1335,10 @@
     <t>students buck</t>
   </si>
   <si>
-    <t>states of</t>
-  </si>
-  <si>
-    <t>statement by</t>
+    <t>states america</t>
+  </si>
+  <si>
+    <t>statement donald</t>
   </si>
   <si>
     <t>special session</t>
@@ -1362,6 +1350,18 @@
     <t>sens johnson</t>
   </si>
   <si>
+    <t>school students</t>
+  </si>
+  <si>
+    <t>ron desantis</t>
+  </si>
+  <si>
+    <t>report card</t>
+  </si>
+  <si>
+    <t>release opportunity</t>
+  </si>
+  <si>
     <t>youngkin incompetence continues</t>
   </si>
   <si>
@@ -1371,40 +1371,28 @@
     <t>white students persist</t>
   </si>
   <si>
-    <t>warrants as valid</t>
-  </si>
-  <si>
-    <t>valid proof of</t>
-  </si>
-  <si>
-    <t>united states of</t>
-  </si>
-  <si>
-    <t>tsa from accepting</t>
+    <t>warrants valid proof</t>
+  </si>
+  <si>
+    <t>valid proof id</t>
+  </si>
+  <si>
+    <t>united states america</t>
+  </si>
+  <si>
+    <t>tsa accepting arrest</t>
   </si>
   <si>
     <t>trump 45th president</t>
   </si>
   <si>
-    <t>trends in national</t>
-  </si>
-  <si>
-    <t>to prohibit tsa</t>
-  </si>
-  <si>
-    <t>to hurt the</t>
-  </si>
-  <si>
-    <t>the united states</t>
+    <t>trends national report</t>
   </si>
   <si>
     <t>students buck national</t>
   </si>
   <si>
-    <t>states of america</t>
-  </si>
-  <si>
-    <t>statement by donald</t>
+    <t>statement donald trump</t>
   </si>
   <si>
     <t>special session governor</t>
@@ -1422,43 +1410,40 @@
     <t>ron desantis faith</t>
   </si>
   <si>
-    <t>youngkin incompetence continues to</t>
+    <t>report card release</t>
+  </si>
+  <si>
+    <t>release opportunity gaps</t>
+  </si>
+  <si>
+    <t>prohibit tsa accepting</t>
+  </si>
+  <si>
+    <t>president united states</t>
+  </si>
+  <si>
+    <t>youngkin incompetence continues hurt</t>
   </si>
   <si>
     <t>wisconsin elementary school students</t>
   </si>
   <si>
-    <t>warrants as valid proof</t>
-  </si>
-  <si>
-    <t>valid proof of id</t>
-  </si>
-  <si>
-    <t>united states of america</t>
-  </si>
-  <si>
-    <t>tsa from accepting arrest</t>
-  </si>
-  <si>
-    <t>trump 45th president of</t>
-  </si>
-  <si>
-    <t>trends in national report</t>
-  </si>
-  <si>
-    <t>to prohibit tsa from</t>
-  </si>
-  <si>
-    <t>to hurt the commonwealt</t>
-  </si>
-  <si>
-    <t>the united states of</t>
+    <t>warrants valid proof id</t>
+  </si>
+  <si>
+    <t>tsa accepting arrest warrants</t>
+  </si>
+  <si>
+    <t>trump 45th president united</t>
+  </si>
+  <si>
+    <t>trends national report card</t>
   </si>
   <si>
     <t>students buck national trends</t>
   </si>
   <si>
-    <t>statement by donald trump</t>
+    <t>statement donald trump 45th</t>
   </si>
   <si>
     <t>special session governor youngkin</t>
@@ -1479,37 +1464,43 @@
     <t>report card release opportunity</t>
   </si>
   <si>
-    <t>release opportunity gaps between</t>
-  </si>
-  <si>
-    <t>youngkin incompetence continues to hurt</t>
+    <t>release opportunity gaps black</t>
+  </si>
+  <si>
+    <t>prohibit tsa accepting arrest</t>
+  </si>
+  <si>
+    <t>president united states america</t>
+  </si>
+  <si>
+    <t>portman introduce legislation prohibit</t>
+  </si>
+  <si>
+    <t>pedro pans biden border</t>
+  </si>
+  <si>
+    <t>pans biden border crisis</t>
+  </si>
+  <si>
+    <t>youngkin incompetence continues hurt commonwealt</t>
   </si>
   <si>
     <t>wisconsin elementary school students buck</t>
   </si>
   <si>
-    <t>warrants as valid proof of</t>
-  </si>
-  <si>
-    <t>tsa from accepting arrest warrants</t>
-  </si>
-  <si>
-    <t>trump 45th president of the</t>
-  </si>
-  <si>
-    <t>trends in national report card</t>
-  </si>
-  <si>
-    <t>to prohibit tsa from accepting</t>
-  </si>
-  <si>
-    <t>the united states of america</t>
-  </si>
-  <si>
-    <t>students buck national trends in</t>
-  </si>
-  <si>
-    <t>statement by donald trump 45th</t>
+    <t>tsa accepting arrest warrants valid</t>
+  </si>
+  <si>
+    <t>trump 45th president united states</t>
+  </si>
+  <si>
+    <t>trends national report card release</t>
+  </si>
+  <si>
+    <t>students buck national trends national</t>
+  </si>
+  <si>
+    <t>statement donald trump 45th president</t>
   </si>
   <si>
     <t>special session governor youngkin incompetence</t>
@@ -1524,22 +1515,31 @@
     <t>school students buck national trends</t>
   </si>
   <si>
-    <t>ron desantis faith leaders and</t>
+    <t>ron desantis faith leaders pedro</t>
   </si>
   <si>
     <t>report card release opportunity gaps</t>
   </si>
   <si>
-    <t>release opportunity gaps between black</t>
-  </si>
-  <si>
-    <t>prohibit tsa from accepting arrest</t>
-  </si>
-  <si>
-    <t>president of the united states</t>
-  </si>
-  <si>
-    <t>portman introduce legislation to prohibit</t>
+    <t>release opportunity gaps black white</t>
+  </si>
+  <si>
+    <t>prohibit tsa accepting arrest warrants</t>
+  </si>
+  <si>
+    <t>portman introduce legislation prohibit tsa</t>
+  </si>
+  <si>
+    <t>pedro pans biden border crisis</t>
+  </si>
+  <si>
+    <t>pans biden border crisis harming</t>
+  </si>
+  <si>
+    <t>opportunity gaps black white students</t>
+  </si>
+  <si>
+    <t>national trends national report card</t>
   </si>
   <si>
     <t>watch</t>
@@ -1569,16 +1569,10 @@
     <t>tour events</t>
   </si>
   <si>
-    <t>to geofence</t>
-  </si>
-  <si>
     <t>state book</t>
   </si>
   <si>
-    <t>ron out</t>
-  </si>
-  <si>
-    <t>of state</t>
+    <t>ron state</t>
   </si>
   <si>
     <t>launching ads</t>
@@ -1593,31 +1587,22 @@
     <t>book tour</t>
   </si>
   <si>
-    <t>ads to</t>
+    <t>ads geofence</t>
   </si>
   <si>
     <t>watch launching ads</t>
   </si>
   <si>
-    <t>to geofence ron</t>
-  </si>
-  <si>
     <t>state book tour</t>
   </si>
   <si>
-    <t>ron out of</t>
-  </si>
-  <si>
-    <t>out of state</t>
-  </si>
-  <si>
-    <t>of state book</t>
-  </si>
-  <si>
-    <t>launching ads to</t>
-  </si>
-  <si>
-    <t>geofence ron out</t>
+    <t>ron state book</t>
+  </si>
+  <si>
+    <t>launching ads geofence</t>
+  </si>
+  <si>
+    <t>geofence ron state</t>
   </si>
   <si>
     <t>desantis watch launching</t>
@@ -1626,64 +1611,46 @@
     <t>book tour events</t>
   </si>
   <si>
-    <t>ads to geofence</t>
-  </si>
-  <si>
-    <t>watch launching ads to</t>
-  </si>
-  <si>
-    <t>to geofence ron out</t>
+    <t>ads geofence ron</t>
+  </si>
+  <si>
+    <t>watch launching ads geofence</t>
   </si>
   <si>
     <t>state book tour events</t>
   </si>
   <si>
-    <t>ron out of state</t>
-  </si>
-  <si>
-    <t>out of state book</t>
-  </si>
-  <si>
-    <t>of state book tour</t>
-  </si>
-  <si>
-    <t>launching ads to geofence</t>
-  </si>
-  <si>
-    <t>geofence ron out of</t>
+    <t>ron state book tour</t>
+  </si>
+  <si>
+    <t>launching ads geofence ron</t>
+  </si>
+  <si>
+    <t>geofence ron state book</t>
   </si>
   <si>
     <t>desantis watch launching ads</t>
   </si>
   <si>
-    <t>ads to geofence ron</t>
-  </si>
-  <si>
-    <t>watch launching ads to geofence</t>
-  </si>
-  <si>
-    <t>to geofence ron out of</t>
-  </si>
-  <si>
-    <t>ron out of state book</t>
-  </si>
-  <si>
-    <t>out of state book tour</t>
-  </si>
-  <si>
-    <t>of state book tour events</t>
-  </si>
-  <si>
-    <t>launching ads to geofence ron</t>
-  </si>
-  <si>
-    <t>geofence ron out of state</t>
-  </si>
-  <si>
-    <t>desantis watch launching ads to</t>
-  </si>
-  <si>
-    <t>ads to geofence ron out</t>
+    <t>ads geofence ron state</t>
+  </si>
+  <si>
+    <t>watch launching ads geofence ron</t>
+  </si>
+  <si>
+    <t>ron state book tour events</t>
+  </si>
+  <si>
+    <t>launching ads geofence ron state</t>
+  </si>
+  <si>
+    <t>geofence ron state book tour</t>
+  </si>
+  <si>
+    <t>desantis watch launching ads geofence</t>
+  </si>
+  <si>
+    <t>ads geofence ron state book</t>
   </si>
   <si>
     <t>york</t>
@@ -1755,10 +1722,7 @@
     <t>witch hunt</t>
   </si>
   <si>
-    <t>trump on</t>
-  </si>
-  <si>
-    <t>to make</t>
+    <t>trump crooked</t>
   </si>
   <si>
     <t>tillis blackburn</t>
@@ -1767,7 +1731,7 @@
     <t>strong global</t>
   </si>
   <si>
-    <t>statement from</t>
+    <t>statement president</t>
   </si>
   <si>
     <t>roads federal</t>
@@ -1782,15 +1746,12 @@
     <t>president donald</t>
   </si>
   <si>
-    <t>position as</t>
+    <t>position strong</t>
   </si>
   <si>
     <t>policy reclaiming</t>
   </si>
   <si>
-    <t>on crooked</t>
-  </si>
-  <si>
     <t>new york</t>
   </si>
   <si>
@@ -1806,16 +1767,19 @@
     <t>global leader</t>
   </si>
   <si>
-    <t>from president</t>
+    <t>foreign policy</t>
+  </si>
+  <si>
+    <t>federal crime</t>
+  </si>
+  <si>
+    <t>donald trump</t>
   </si>
   <si>
     <t>york ag witch</t>
   </si>
   <si>
-    <t>trump on crooked</t>
-  </si>
-  <si>
-    <t>to make blocking</t>
+    <t>trump crooked joe</t>
   </si>
   <si>
     <t>tillis blackburn introduce</t>
@@ -1824,7 +1788,7 @@
     <t>strong global leader</t>
   </si>
   <si>
-    <t>statement from president</t>
+    <t>statement president donald</t>
   </si>
   <si>
     <t>roads federal crime</t>
@@ -1839,15 +1803,12 @@
     <t>president donald trump</t>
   </si>
   <si>
-    <t>position as strong</t>
+    <t>position strong global</t>
   </si>
   <si>
     <t>policy reclaiming america</t>
   </si>
   <si>
-    <t>on crooked joe</t>
-  </si>
-  <si>
     <t>new york ag</t>
   </si>
   <si>
@@ -1857,51 +1818,51 @@
     <t>joe biden directed</t>
   </si>
   <si>
-    <t>introduce bill to</t>
-  </si>
-  <si>
-    <t>from president donald</t>
+    <t>introduce bill make</t>
   </si>
   <si>
     <t>foreign policy reclaiming</t>
   </si>
   <si>
-    <t>donald trump on</t>
+    <t>donald trump crooked</t>
+  </si>
+  <si>
+    <t>directed new york</t>
+  </si>
+  <si>
+    <t>crooked joe biden</t>
+  </si>
+  <si>
+    <t>blocking public roads</t>
   </si>
   <si>
     <t>york ag witch hunt</t>
   </si>
   <si>
-    <t>trump on crooked joe</t>
-  </si>
-  <si>
-    <t>to make blocking public</t>
+    <t>trump crooked joe biden</t>
   </si>
   <si>
     <t>tillis blackburn introduce bill</t>
   </si>
   <si>
-    <t>statement from president donald</t>
-  </si>
-  <si>
-    <t>reclaiming america position as</t>
+    <t>statement president donald trump</t>
+  </si>
+  <si>
+    <t>reclaiming america position strong</t>
   </si>
   <si>
     <t>public roads federal crime</t>
   </si>
   <si>
-    <t>president donald trump on</t>
-  </si>
-  <si>
-    <t>position as strong global</t>
+    <t>president donald trump crooked</t>
+  </si>
+  <si>
+    <t>position strong global leader</t>
   </si>
   <si>
     <t>policy reclaiming america position</t>
   </si>
   <si>
-    <t>on crooked joe biden</t>
-  </si>
-  <si>
     <t>new york ag witch</t>
   </si>
   <si>
@@ -1911,16 +1872,13 @@
     <t>joe biden directed new</t>
   </si>
   <si>
-    <t>introduce bill to make</t>
-  </si>
-  <si>
-    <t>from president donald trump</t>
+    <t>introduce bill make blocking</t>
   </si>
   <si>
     <t>foreign policy reclaiming america</t>
   </si>
   <si>
-    <t>donald trump on crooked</t>
+    <t>donald trump crooked joe</t>
   </si>
   <si>
     <t>directed new york ag</t>
@@ -1929,31 +1887,31 @@
     <t>crooked joe biden directed</t>
   </si>
   <si>
-    <t>trump on crooked joe biden</t>
-  </si>
-  <si>
-    <t>to make blocking public roads</t>
-  </si>
-  <si>
-    <t>tillis blackburn introduce bill to</t>
-  </si>
-  <si>
-    <t>statement from president donald trump</t>
-  </si>
-  <si>
-    <t>reclaiming america position as strong</t>
-  </si>
-  <si>
-    <t>president donald trump on crooked</t>
-  </si>
-  <si>
-    <t>position as strong global leader</t>
-  </si>
-  <si>
-    <t>policy reclaiming america position as</t>
-  </si>
-  <si>
-    <t>on crooked joe biden directed</t>
+    <t>blocking public roads federal</t>
+  </si>
+  <si>
+    <t>blackburn introduce bill make</t>
+  </si>
+  <si>
+    <t>bill make blocking public</t>
+  </si>
+  <si>
+    <t>trump crooked joe biden directed</t>
+  </si>
+  <si>
+    <t>tillis blackburn introduce bill make</t>
+  </si>
+  <si>
+    <t>statement president donald trump crooked</t>
+  </si>
+  <si>
+    <t>reclaiming america position strong global</t>
+  </si>
+  <si>
+    <t>president donald trump crooked joe</t>
+  </si>
+  <si>
+    <t>policy reclaiming america position strong</t>
   </si>
   <si>
     <t>new york ag witch hunt</t>
@@ -1965,16 +1923,13 @@
     <t>joe biden directed new york</t>
   </si>
   <si>
-    <t>introduce bill to make blocking</t>
-  </si>
-  <si>
-    <t>from president donald trump on</t>
+    <t>introduce bill make blocking public</t>
   </si>
   <si>
     <t>foreign policy reclaiming america position</t>
   </si>
   <si>
-    <t>donald trump on crooked joe</t>
+    <t>donald trump crooked joe biden</t>
   </si>
   <si>
     <t>directed new york ag witch</t>
@@ -1986,7 +1941,16 @@
     <t>blocking public roads federal crime</t>
   </si>
   <si>
-    <t>blackburn introduce bill to make</t>
+    <t>blackburn introduce bill make blocking</t>
+  </si>
+  <si>
+    <t>bill make blocking public roads</t>
+  </si>
+  <si>
+    <t>biden directed new york ag</t>
+  </si>
+  <si>
+    <t>america position strong global leader</t>
   </si>
 </sst>
 </file>
@@ -2952,7 +2916,7 @@
         <v>56</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2963,7 +2927,7 @@
         <v>57</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -3161,7 +3125,7 @@
         <v>75</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -3370,7 +3334,7 @@
         <v>94</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -3579,7 +3543,7 @@
         <v>113</v>
       </c>
       <c r="C112">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -8160,7 +8124,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8388,7 +8352,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>523</v>
@@ -8399,7 +8363,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>524</v>
@@ -8476,7 +8440,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
         <v>531</v>
@@ -8487,7 +8451,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
         <v>532</v>
@@ -8498,7 +8462,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
         <v>533</v>
@@ -8509,7 +8473,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
         <v>534</v>
@@ -8520,7 +8484,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
         <v>535</v>
@@ -8553,7 +8517,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
         <v>538</v>
@@ -8564,7 +8528,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
         <v>539</v>
@@ -8575,7 +8539,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
         <v>540</v>
@@ -8586,7 +8550,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
         <v>541</v>
@@ -8597,7 +8561,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
         <v>542</v>
@@ -8608,133 +8572,12 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
         <v>543</v>
       </c>
       <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42">
-        <v>4</v>
-      </c>
-      <c r="B42" t="s">
-        <v>544</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>545</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44">
-        <v>5</v>
-      </c>
-      <c r="B44" t="s">
-        <v>546</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45">
-        <v>5</v>
-      </c>
-      <c r="B45" t="s">
-        <v>547</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46">
-        <v>5</v>
-      </c>
-      <c r="B46" t="s">
-        <v>548</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47">
-        <v>5</v>
-      </c>
-      <c r="B47" t="s">
-        <v>549</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48">
-        <v>5</v>
-      </c>
-      <c r="B48" t="s">
-        <v>550</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49">
-        <v>5</v>
-      </c>
-      <c r="B49" t="s">
-        <v>551</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50">
-        <v>5</v>
-      </c>
-      <c r="B50" t="s">
-        <v>552</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51">
-        <v>5</v>
-      </c>
-      <c r="B51" t="s">
-        <v>553</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52">
-        <v>5</v>
-      </c>
-      <c r="B52" t="s">
-        <v>554</v>
-      </c>
-      <c r="C52">
         <v>1</v>
       </c>
     </row>
@@ -8745,7 +8588,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8767,7 +8610,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -8778,7 +8621,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -8800,7 +8643,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -8833,7 +8676,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -8844,7 +8687,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -8877,7 +8720,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -8888,7 +8731,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -8910,7 +8753,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -8921,7 +8764,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>563</v>
+        <v>552</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -8932,7 +8775,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>564</v>
+        <v>553</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -8954,7 +8797,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -8965,7 +8808,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -8976,7 +8819,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -9009,7 +8852,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -9020,7 +8863,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>569</v>
+        <v>558</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -9031,7 +8874,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>570</v>
+        <v>559</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -9042,7 +8885,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -9053,7 +8896,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -9064,7 +8907,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -9086,7 +8929,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -9097,7 +8940,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -9108,7 +8951,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -9119,7 +8962,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -9130,7 +8973,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -9141,7 +8984,7 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>579</v>
+        <v>568</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -9152,7 +8995,7 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -9163,7 +9006,7 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -9174,7 +9017,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -9185,7 +9028,7 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -9196,7 +9039,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -9207,7 +9050,7 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -9218,7 +9061,7 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -9229,7 +9072,7 @@
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -9240,7 +9083,7 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -9251,7 +9094,7 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -9262,7 +9105,7 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -9273,7 +9116,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -9284,7 +9127,7 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -9295,7 +9138,7 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -9306,7 +9149,7 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -9317,7 +9160,7 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -9328,7 +9171,7 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -9339,7 +9182,7 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -9350,7 +9193,7 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -9361,7 +9204,7 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -9372,7 +9215,7 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -9383,7 +9226,7 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -9394,7 +9237,7 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -9405,7 +9248,7 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>603</v>
+        <v>592</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -9416,7 +9259,7 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -9427,7 +9270,7 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -9438,7 +9281,7 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -9449,7 +9292,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -9460,7 +9303,7 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>608</v>
+        <v>597</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -9471,7 +9314,7 @@
         <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -9482,7 +9325,7 @@
         <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>610</v>
+        <v>599</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -9493,7 +9336,7 @@
         <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -9504,7 +9347,7 @@
         <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -9515,7 +9358,7 @@
         <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -9526,7 +9369,7 @@
         <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>614</v>
+        <v>603</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -9537,7 +9380,7 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -9548,7 +9391,7 @@
         <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -9559,7 +9402,7 @@
         <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -9570,7 +9413,7 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -9581,7 +9424,7 @@
         <v>4</v>
       </c>
       <c r="B76" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -9592,7 +9435,7 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -9603,7 +9446,7 @@
         <v>4</v>
       </c>
       <c r="B78" t="s">
-        <v>621</v>
+        <v>610</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -9614,7 +9457,7 @@
         <v>4</v>
       </c>
       <c r="B79" t="s">
-        <v>622</v>
+        <v>611</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -9625,7 +9468,7 @@
         <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>623</v>
+        <v>612</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -9636,7 +9479,7 @@
         <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>624</v>
+        <v>613</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -9647,7 +9490,7 @@
         <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>625</v>
+        <v>614</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -9658,7 +9501,7 @@
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>626</v>
+        <v>615</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -9669,7 +9512,7 @@
         <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -9680,7 +9523,7 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>628</v>
+        <v>617</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -9691,7 +9534,7 @@
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>629</v>
+        <v>618</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -9702,7 +9545,7 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>630</v>
+        <v>619</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -9713,7 +9556,7 @@
         <v>4</v>
       </c>
       <c r="B88" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -9724,7 +9567,7 @@
         <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>632</v>
+        <v>621</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -9735,7 +9578,7 @@
         <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>633</v>
+        <v>622</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -9746,7 +9589,7 @@
         <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>634</v>
+        <v>623</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -9757,7 +9600,7 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>635</v>
+        <v>624</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -9768,7 +9611,7 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>636</v>
+        <v>625</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -9779,7 +9622,7 @@
         <v>5</v>
       </c>
       <c r="B94" t="s">
-        <v>637</v>
+        <v>626</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -9790,7 +9633,7 @@
         <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>638</v>
+        <v>627</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -9801,7 +9644,7 @@
         <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>639</v>
+        <v>628</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -9812,7 +9655,7 @@
         <v>5</v>
       </c>
       <c r="B97" t="s">
-        <v>640</v>
+        <v>629</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -9823,7 +9666,7 @@
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>641</v>
+        <v>630</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -9834,7 +9677,7 @@
         <v>5</v>
       </c>
       <c r="B99" t="s">
-        <v>642</v>
+        <v>631</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -9845,7 +9688,7 @@
         <v>5</v>
       </c>
       <c r="B100" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -9856,7 +9699,7 @@
         <v>5</v>
       </c>
       <c r="B101" t="s">
-        <v>644</v>
+        <v>633</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -9867,7 +9710,7 @@
         <v>5</v>
       </c>
       <c r="B102" t="s">
-        <v>645</v>
+        <v>634</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -9878,7 +9721,7 @@
         <v>5</v>
       </c>
       <c r="B103" t="s">
-        <v>646</v>
+        <v>635</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -9889,7 +9732,7 @@
         <v>5</v>
       </c>
       <c r="B104" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -9900,7 +9743,7 @@
         <v>5</v>
       </c>
       <c r="B105" t="s">
-        <v>648</v>
+        <v>637</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -9911,7 +9754,7 @@
         <v>5</v>
       </c>
       <c r="B106" t="s">
-        <v>649</v>
+        <v>638</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -9922,7 +9765,7 @@
         <v>5</v>
       </c>
       <c r="B107" t="s">
-        <v>650</v>
+        <v>639</v>
       </c>
       <c r="C107">
         <v>1</v>
@@ -9933,7 +9776,7 @@
         <v>5</v>
       </c>
       <c r="B108" t="s">
-        <v>651</v>
+        <v>640</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -9944,7 +9787,7 @@
         <v>5</v>
       </c>
       <c r="B109" t="s">
-        <v>652</v>
+        <v>641</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -9955,7 +9798,7 @@
         <v>5</v>
       </c>
       <c r="B110" t="s">
-        <v>653</v>
+        <v>642</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -9966,20 +9809,9 @@
         <v>5</v>
       </c>
       <c r="B111" t="s">
-        <v>654</v>
+        <v>643</v>
       </c>
       <c r="C111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112">
-        <v>5</v>
-      </c>
-      <c r="B112" t="s">
-        <v>655</v>
-      </c>
-      <c r="C112">
         <v>1</v>
       </c>
     </row>

</xml_diff>